<commit_message>
ER optimal and calculate new temporal using the MX_ diff database
</commit_message>
<xml_diff>
--- a/document/er_memory.xlsx
+++ b/document/er_memory.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>memory</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>average waiting time</t>
   </si>
@@ -96,38 +93,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -138,11 +104,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>memory</c:v>
+                  <c:v>average waiting time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -159,7 +125,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
@@ -194,40 +160,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E63A-40AA-BC17-96DA149545CA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>average waiting time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$10</c:f>
@@ -267,7 +200,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E63A-40AA-BC17-96DA149545CA}"/>
+              <c16:uniqueId val="{00000000-5B9E-4C82-9F50-6C5149A56FE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -280,16 +213,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="344000815"/>
-        <c:axId val="344008303"/>
+        <c:axId val="1543104767"/>
+        <c:axId val="1543105183"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344000815"/>
+        <c:axId val="1543104767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -326,7 +260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344008303"/>
+        <c:crossAx val="1543105183"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -334,9 +268,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344008303"/>
+        <c:axId val="1543105183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -385,7 +320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344000815"/>
+        <c:crossAx val="1543104767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -397,38 +332,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1026,20 +929,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1323,7 +1226,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,14 +1235,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update draft, recalculate GR risk for most scenario, finish walking and ER memory. To do: calculate average and recalculate NR
</commit_message>
<xml_diff>
--- a/document/er_memory.xlsx
+++ b/document/er_memory.xlsx
@@ -95,7 +95,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11592825896762905"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.85351618547681551"/>
+          <c:h val="0.78054024496937879"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -223,6 +233,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory period</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.80666666666666664"/>
+              <c:y val="0.92497666958296876"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -289,6 +362,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Waiting</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1226,7 +1360,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>